<commit_message>
renamed truncated_prediction back to price
</commit_message>
<xml_diff>
--- a/data_spring_2025.xlsx
+++ b/data_spring_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekgibbs/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFAE3D9-3BFE-F844-A922-62593DD87169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89849DE9-7A53-CB47-A3B6-6E5BC74724A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32680" yWindow="-660" windowWidth="28800" windowHeight="17500" xr2:uid="{26079AD5-63BA-6C45-88C1-5844B765A22E}"/>
   </bookViews>
@@ -1595,13 +1595,13 @@
     <t>uniqueid</t>
   </si>
   <si>
-    <t>Truncated_prediction</t>
-  </si>
-  <si>
     <t>SELECTED_MEAN</t>
   </si>
   <si>
     <t>SELECTED_STDEV</t>
+  </si>
+  <si>
+    <t>price</t>
   </si>
 </sst>
 </file>
@@ -2047,7 +2047,7 @@
   <dimension ref="A1:P236"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2099,13 +2099,13 @@
         <v>516</v>
       </c>
       <c r="N1" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>518</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>519</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
data: update column names to price_predicted, resid_mean, and resid_stdev
</commit_message>
<xml_diff>
--- a/data_spring_2025.xlsx
+++ b/data_spring_2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekgibbs/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ohkwo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89849DE9-7A53-CB47-A3B6-6E5BC74724A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F110DE6C-F131-45C4-BF5F-7578F74CF048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32680" yWindow="-660" windowWidth="28800" windowHeight="17500" xr2:uid="{26079AD5-63BA-6C45-88C1-5844B765A22E}"/>
+    <workbookView xWindow="57405" yWindow="-195" windowWidth="29190" windowHeight="15870" xr2:uid="{26079AD5-63BA-6C45-88C1-5844B765A22E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -1595,24 +1595,27 @@
     <t>uniqueid</t>
   </si>
   <si>
-    <t>SELECTED_MEAN</t>
-  </si>
-  <si>
-    <t>SELECTED_STDEV</t>
-  </si>
-  <si>
-    <t>price</t>
+    <t>price_predicted</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>resid_mean</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>resid_stdev</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1620,14 +1623,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1642,6 +1645,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1710,8 +1720,8 @@
     <xf numFmtId="1" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{3AF1E909-AFE2-E44A-95DF-48B5C824B6F1}"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1727,7 +1737,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2046,11 +2056,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P236"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="19.149999999999999" x14ac:dyDescent="0.7"/>
   <cols>
     <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="61.83203125" customWidth="1"/>
@@ -2058,7 +2068,7 @@
     <col min="15" max="16" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A1" t="s">
         <v>517</v>
       </c>
@@ -2099,16 +2109,16 @@
         <v>516</v>
       </c>
       <c r="N1" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>519</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>520</v>
       </c>
-      <c r="O1" s="5" t="s">
-        <v>518</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2158,7 +2168,7 @@
         <v>187.85629601860171</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2208,7 +2218,7 @@
         <v>187.85629601860171</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2258,7 +2268,7 @@
         <v>69.677383497541285</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2308,7 +2318,7 @@
         <v>12.788822787019859</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2358,7 +2368,7 @@
         <v>14.329423002786024</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2408,7 +2418,7 @@
         <v>95.814541017578293</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2458,7 +2468,7 @@
         <v>0.66240191388999159</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2508,7 +2518,7 @@
         <v>13.541368215707591</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2558,7 +2568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2608,7 +2618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2658,7 +2668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2708,7 +2718,7 @@
         <v>19.490190931572183</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2758,7 +2768,7 @@
         <v>72.527655943554436</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2808,7 +2818,7 @@
         <v>98.024632730861086</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2858,7 +2868,7 @@
         <v>98.024632730861086</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2908,7 +2918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2958,7 +2968,7 @@
         <v>572.94059204435052</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3008,7 +3018,7 @@
         <v>10.096534354197727</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3058,7 +3068,7 @@
         <v>152.46496622388258</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3108,7 +3118,7 @@
         <v>152.46496622388258</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3158,7 +3168,7 @@
         <v>152.46496622388258</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3208,7 +3218,7 @@
         <v>152.46496622388258</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3258,7 +3268,7 @@
         <v>150.21235569044291</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3308,7 +3318,7 @@
         <v>150.21235569044291</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3358,7 +3368,7 @@
         <v>188.85347479941004</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3408,7 +3418,7 @@
         <v>188.85347479941004</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3458,7 +3468,7 @@
         <v>188.85347479941004</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3508,7 +3518,7 @@
         <v>173.11635705772196</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3558,7 +3568,7 @@
         <v>43.565953405979251</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3608,7 +3618,7 @@
         <v>20.10666435773841</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3658,7 +3668,7 @@
         <v>190.26714217496891</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3708,7 +3718,7 @@
         <v>213.2027705180729</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3758,7 +3768,7 @@
         <v>371.62544551664422</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3808,7 +3818,7 @@
         <v>371.62544551664422</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3858,7 +3868,7 @@
         <v>296.62328358232611</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3908,7 +3918,7 @@
         <v>23.929319081305625</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3958,7 +3968,7 @@
         <v>154.74054380226181</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4008,7 +4018,7 @@
         <v>3.294018845213194</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4058,7 +4068,7 @@
         <v>19.240070923846737</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4108,7 +4118,7 @@
         <v>96.991118362999813</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4158,7 +4168,7 @@
         <v>7.0363675784221149</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4208,7 +4218,7 @@
         <v>123.40783231561922</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4258,7 +4268,7 @@
         <v>1144.7889630647833</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4308,7 +4318,7 @@
         <v>730.88031909695098</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4358,7 +4368,7 @@
         <v>730.88031909695098</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4408,7 +4418,7 @@
         <v>170.61250509646521</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4458,7 +4468,7 @@
         <v>174.42639244868801</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4508,7 +4518,7 @@
         <v>99.038223762679294</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4558,7 +4568,7 @@
         <v>25.566815144068318</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4608,7 +4618,7 @@
         <v>52.225403169542638</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4658,7 +4668,7 @@
         <v>9.5110012039902294</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4708,7 +4718,7 @@
         <v>325.40002518197019</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4758,7 +4768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4808,7 +4818,7 @@
         <v>36.800798497418569</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4858,7 +4868,7 @@
         <v>18.928971087072604</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4908,7 +4918,7 @@
         <v>18.928971087072604</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4958,7 +4968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A59">
         <v>58</v>
       </c>
@@ -5008,7 +5018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5058,7 +5068,7 @@
         <v>18.436815284879675</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A61">
         <v>60</v>
       </c>
@@ -5108,7 +5118,7 @@
         <v>18.436815284879675</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A62">
         <v>61</v>
       </c>
@@ -5158,7 +5168,7 @@
         <v>103.88661220134681</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A63">
         <v>62</v>
       </c>
@@ -5208,7 +5218,7 @@
         <v>0.27783475903992005</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A64">
         <v>63</v>
       </c>
@@ -5258,7 +5268,7 @@
         <v>0.27783475903992005</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A65">
         <v>64</v>
       </c>
@@ -5308,7 +5318,7 @@
         <v>80.596969909588978</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A66">
         <v>65</v>
       </c>
@@ -5358,7 +5368,7 @@
         <v>80.596969909588978</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A67">
         <v>66</v>
       </c>
@@ -5408,7 +5418,7 @@
         <v>115.67324214587806</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A68">
         <v>67</v>
       </c>
@@ -5458,7 +5468,7 @@
         <v>446.1319928661913</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A69">
         <v>68</v>
       </c>
@@ -5508,7 +5518,7 @@
         <v>18.524179172027647</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A70">
         <v>69</v>
       </c>
@@ -5558,7 +5568,7 @@
         <v>48.737731319030019</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A71">
         <v>70</v>
       </c>
@@ -5608,7 +5618,7 @@
         <v>26.324952582138128</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A72">
         <v>71</v>
       </c>
@@ -5658,7 +5668,7 @@
         <v>26.324952582138128</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A73">
         <v>72</v>
       </c>
@@ -5708,7 +5718,7 @@
         <v>12.777632772582971</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A74">
         <v>73</v>
       </c>
@@ -5758,7 +5768,7 @@
         <v>16.872663078637288</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A75">
         <v>74</v>
       </c>
@@ -5808,7 +5818,7 @@
         <v>261.39466715388164</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A76">
         <v>75</v>
       </c>
@@ -5858,7 +5868,7 @@
         <v>80.174174214731394</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A77">
         <v>76</v>
       </c>
@@ -5908,7 +5918,7 @@
         <v>80.174174214731394</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A78">
         <v>77</v>
       </c>
@@ -5958,7 +5968,7 @@
         <v>80.174174214731394</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A79">
         <v>78</v>
       </c>
@@ -6008,7 +6018,7 @@
         <v>241.20882330518251</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A80">
         <v>79</v>
       </c>
@@ -6058,7 +6068,7 @@
         <v>169.9686752282438</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A81">
         <v>80</v>
       </c>
@@ -6108,7 +6118,7 @@
         <v>169.9686752282438</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A82">
         <v>81</v>
       </c>
@@ -6158,7 +6168,7 @@
         <v>48.271229796021053</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A83">
         <v>82</v>
       </c>
@@ -6208,7 +6218,7 @@
         <v>211.17896898690555</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A84">
         <v>83</v>
       </c>
@@ -6258,7 +6268,7 @@
         <v>91.759092535678974</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A85">
         <v>84</v>
       </c>
@@ -6308,7 +6318,7 @@
         <v>104.75664921941434</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A86">
         <v>85</v>
       </c>
@@ -6358,7 +6368,7 @@
         <v>104.75664921941434</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A87">
         <v>86</v>
       </c>
@@ -6408,7 +6418,7 @@
         <v>93.138969238199834</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A88">
         <v>87</v>
       </c>
@@ -6458,7 +6468,7 @@
         <v>93.138969238199834</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A89">
         <v>88</v>
       </c>
@@ -6508,7 +6518,7 @@
         <v>188.30512932785297</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A90">
         <v>89</v>
       </c>
@@ -6558,7 +6568,7 @@
         <v>188.30512932785297</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A91">
         <v>90</v>
       </c>
@@ -6608,7 +6618,7 @@
         <v>54.143273308685202</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A92">
         <v>91</v>
       </c>
@@ -6658,7 +6668,7 @@
         <v>54.143273308685202</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A93">
         <v>92</v>
       </c>
@@ -6708,7 +6718,7 @@
         <v>18.920062805255025</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A94">
         <v>93</v>
       </c>
@@ -6758,7 +6768,7 @@
         <v>259.3166564993341</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A95">
         <v>94</v>
       </c>
@@ -6808,7 +6818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A96">
         <v>95</v>
       </c>
@@ -6858,7 +6868,7 @@
         <v>65.281042129317299</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A97">
         <v>96</v>
       </c>
@@ -6908,7 +6918,7 @@
         <v>34.812734900599509</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A98">
         <v>97</v>
       </c>
@@ -6958,7 +6968,7 @@
         <v>18.366683446465178</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A99">
         <v>98</v>
       </c>
@@ -7008,7 +7018,7 @@
         <v>137.54950151096202</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A100">
         <v>99</v>
       </c>
@@ -7058,7 +7068,7 @@
         <v>106.02843115730522</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A101">
         <v>100</v>
       </c>
@@ -7108,7 +7118,7 @@
         <v>106.02843115730522</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A102">
         <v>101</v>
       </c>
@@ -7158,7 +7168,7 @@
         <v>138.35026109605252</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A103">
         <v>102</v>
       </c>
@@ -7208,7 +7218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A104">
         <v>103</v>
       </c>
@@ -7258,7 +7268,7 @@
         <v>123.73724902818223</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A105">
         <v>104</v>
       </c>
@@ -7308,7 +7318,7 @@
         <v>123.73724902818223</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A106">
         <v>105</v>
       </c>
@@ -7358,7 +7368,7 @@
         <v>96.809026739429655</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A107">
         <v>106</v>
       </c>
@@ -7408,7 +7418,7 @@
         <v>1101.0993426578223</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A108">
         <v>107</v>
       </c>
@@ -7458,7 +7468,7 @@
         <v>520.82834985954548</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A109">
         <v>108</v>
       </c>
@@ -7508,7 +7518,7 @@
         <v>263.64673625310365</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A110">
         <v>109</v>
       </c>
@@ -7558,7 +7568,7 @@
         <v>520.82834985954548</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A111">
         <v>110</v>
       </c>
@@ -7608,7 +7618,7 @@
         <v>87.728926191497962</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A112">
         <v>111</v>
       </c>
@@ -7658,7 +7668,7 @@
         <v>87.728926191497962</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A113">
         <v>112</v>
       </c>
@@ -7708,7 +7718,7 @@
         <v>103.05004286573133</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A114">
         <v>113</v>
       </c>
@@ -7758,7 +7768,7 @@
         <v>14.694960386981737</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A115">
         <v>114</v>
       </c>
@@ -7808,7 +7818,7 @@
         <v>14.694960386981737</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A116">
         <v>115</v>
       </c>
@@ -7858,7 +7868,7 @@
         <v>57.96398751183127</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A117">
         <v>116</v>
       </c>
@@ -7908,7 +7918,7 @@
         <v>314.70654544373429</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A118">
         <v>117</v>
       </c>
@@ -7958,7 +7968,7 @@
         <v>79.0363573472588</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A119">
         <v>118</v>
       </c>
@@ -8008,7 +8018,7 @@
         <v>2.3264379434151095</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A120">
         <v>119</v>
       </c>
@@ -8058,7 +8068,7 @@
         <v>49.248314296454197</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A121">
         <v>120</v>
       </c>
@@ -8108,7 +8118,7 @@
         <v>49.248314296454197</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A122">
         <v>121</v>
       </c>
@@ -8158,7 +8168,7 @@
         <v>318.20381710210626</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A123">
         <v>122</v>
       </c>
@@ -8208,7 +8218,7 @@
         <v>131.45538018500218</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A124">
         <v>123</v>
       </c>
@@ -8258,7 +8268,7 @@
         <v>82.3757002893378</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A125">
         <v>124</v>
       </c>
@@ -8308,7 +8318,7 @@
         <v>131.45538018500218</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A126">
         <v>125</v>
       </c>
@@ -8358,7 +8368,7 @@
         <v>82.3757002893378</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A127">
         <v>126</v>
       </c>
@@ -8408,7 +8418,7 @@
         <v>53.503919278011473</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A128">
         <v>127</v>
       </c>
@@ -8458,7 +8468,7 @@
         <v>53.503919278011473</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A129">
         <v>128</v>
       </c>
@@ -8508,7 +8518,7 @@
         <v>53.503919278011473</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A130">
         <v>129</v>
       </c>
@@ -8558,7 +8568,7 @@
         <v>53.503919278011473</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A131">
         <v>130</v>
       </c>
@@ -8608,7 +8618,7 @@
         <v>22.754301285846644</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A132">
         <v>131</v>
       </c>
@@ -8658,7 +8668,7 @@
         <v>22.754301285846644</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A133">
         <v>132</v>
       </c>
@@ -8708,7 +8718,7 @@
         <v>103.5616923455884</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A134">
         <v>133</v>
       </c>
@@ -8758,7 +8768,7 @@
         <v>130.71105437410361</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A135">
         <v>134</v>
       </c>
@@ -8808,7 +8818,7 @@
         <v>356.14234564152707</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A136">
         <v>135</v>
       </c>
@@ -8858,7 +8868,7 @@
         <v>90.234889371301605</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A137">
         <v>136</v>
       </c>
@@ -8908,7 +8918,7 @@
         <v>13.722436987272076</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A138">
         <v>137</v>
       </c>
@@ -8958,7 +8968,7 @@
         <v>135.27057278252303</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A139">
         <v>138</v>
       </c>
@@ -9008,7 +9018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A140">
         <v>139</v>
       </c>
@@ -9058,7 +9068,7 @@
         <v>50.42006629945233</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A141">
         <v>140</v>
       </c>
@@ -9108,7 +9118,7 @@
         <v>18.990840069725987</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A142">
         <v>141</v>
       </c>
@@ -9158,7 +9168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A143">
         <v>142</v>
       </c>
@@ -9208,7 +9218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A144">
         <v>143</v>
       </c>
@@ -9258,7 +9268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A145">
         <v>144</v>
       </c>
@@ -9308,7 +9318,7 @@
         <v>298.24820329640636</v>
       </c>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A146">
         <v>145</v>
       </c>
@@ -9358,7 +9368,7 @@
         <v>298.24820329640636</v>
       </c>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A147">
         <v>146</v>
       </c>
@@ -9408,7 +9418,7 @@
         <v>298.24820329640636</v>
       </c>
     </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A148">
         <v>147</v>
       </c>
@@ -9458,7 +9468,7 @@
         <v>93.067431965380862</v>
       </c>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A149">
         <v>148</v>
       </c>
@@ -9508,7 +9518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A150">
         <v>149</v>
       </c>
@@ -9558,7 +9568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A151">
         <v>150</v>
       </c>
@@ -9608,7 +9618,7 @@
         <v>107.45943470934107</v>
       </c>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A152">
         <v>151</v>
       </c>
@@ -9658,7 +9668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A153">
         <v>152</v>
       </c>
@@ -9708,7 +9718,7 @@
         <v>332.69136322539259</v>
       </c>
     </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A154">
         <v>153</v>
       </c>
@@ -9758,7 +9768,7 @@
         <v>377.6316994998395</v>
       </c>
     </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A155">
         <v>154</v>
       </c>
@@ -9808,7 +9818,7 @@
         <v>377.6316994998395</v>
       </c>
     </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A156">
         <v>155</v>
       </c>
@@ -9858,7 +9868,7 @@
         <v>377.6316994998395</v>
       </c>
     </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A157">
         <v>156</v>
       </c>
@@ -9908,7 +9918,7 @@
         <v>40.931994413510886</v>
       </c>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A158">
         <v>157</v>
       </c>
@@ -9958,7 +9968,7 @@
         <v>40.931994413510886</v>
       </c>
     </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A159">
         <v>158</v>
       </c>
@@ -10008,7 +10018,7 @@
         <v>259.92588365930123</v>
       </c>
     </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A160">
         <v>159</v>
       </c>
@@ -10058,7 +10068,7 @@
         <v>259.92588365930123</v>
       </c>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A161">
         <v>160</v>
       </c>
@@ -10108,7 +10118,7 @@
         <v>50.392975351545083</v>
       </c>
     </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A162">
         <v>161</v>
       </c>
@@ -10158,7 +10168,7 @@
         <v>76.012850017808816</v>
       </c>
     </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A163">
         <v>162</v>
       </c>
@@ -10208,7 +10218,7 @@
         <v>48.78990210789744</v>
       </c>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A164">
         <v>163</v>
       </c>
@@ -10258,7 +10268,7 @@
         <v>80.979274002535888</v>
       </c>
     </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A165">
         <v>164</v>
       </c>
@@ -10308,7 +10318,7 @@
         <v>50.392975351545083</v>
       </c>
     </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A166">
         <v>165</v>
       </c>
@@ -10358,7 +10368,7 @@
         <v>76.012850017808816</v>
       </c>
     </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A167">
         <v>166</v>
       </c>
@@ -10408,7 +10418,7 @@
         <v>48.78990210789744</v>
       </c>
     </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A168">
         <v>167</v>
       </c>
@@ -10458,7 +10468,7 @@
         <v>80.979274002535888</v>
       </c>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A169">
         <v>168</v>
       </c>
@@ -10508,7 +10518,7 @@
         <v>91.018472494869343</v>
       </c>
     </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A170">
         <v>169</v>
       </c>
@@ -10558,7 +10568,7 @@
         <v>91.018472494869343</v>
       </c>
     </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A171">
         <v>170</v>
       </c>
@@ -10608,7 +10618,7 @@
         <v>41.580182454058182</v>
       </c>
     </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A172">
         <v>171</v>
       </c>
@@ -10658,7 +10668,7 @@
         <v>311.48953288356205</v>
       </c>
     </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A173">
         <v>172</v>
       </c>
@@ -10708,7 +10718,7 @@
         <v>203.05985273917642</v>
       </c>
     </row>
-    <row r="174" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A174">
         <v>173</v>
       </c>
@@ -10758,7 +10768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A175">
         <v>174</v>
       </c>
@@ -10808,7 +10818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A176">
         <v>175</v>
       </c>
@@ -10858,7 +10868,7 @@
         <v>39.584827029335791</v>
       </c>
     </row>
-    <row r="177" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A177">
         <v>176</v>
       </c>
@@ -10908,7 +10918,7 @@
         <v>39.584827029335791</v>
       </c>
     </row>
-    <row r="178" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A178">
         <v>177</v>
       </c>
@@ -10958,7 +10968,7 @@
         <v>244.16151470567286</v>
       </c>
     </row>
-    <row r="179" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A179">
         <v>178</v>
       </c>
@@ -11008,7 +11018,7 @@
         <v>181.53020096084254</v>
       </c>
     </row>
-    <row r="180" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A180">
         <v>179</v>
       </c>
@@ -11058,7 +11068,7 @@
         <v>149.3282051009059</v>
       </c>
     </row>
-    <row r="181" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A181">
         <v>180</v>
       </c>
@@ -11108,7 +11118,7 @@
         <v>149.3282051009059</v>
       </c>
     </row>
-    <row r="182" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A182">
         <v>181</v>
       </c>
@@ -11158,7 +11168,7 @@
         <v>189.98166251719726</v>
       </c>
     </row>
-    <row r="183" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A183">
         <v>182</v>
       </c>
@@ -11208,7 +11218,7 @@
         <v>189.98166251719726</v>
       </c>
     </row>
-    <row r="184" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A184">
         <v>183</v>
       </c>
@@ -11258,7 +11268,7 @@
         <v>189.98166251719726</v>
       </c>
     </row>
-    <row r="185" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A185">
         <v>184</v>
       </c>
@@ -11308,7 +11318,7 @@
         <v>134.49585827054338</v>
       </c>
     </row>
-    <row r="186" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A186">
         <v>185</v>
       </c>
@@ -11358,7 +11368,7 @@
         <v>174.69591896156371</v>
       </c>
     </row>
-    <row r="187" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A187">
         <v>186</v>
       </c>
@@ -11408,7 +11418,7 @@
         <v>5.9768732617588851</v>
       </c>
     </row>
-    <row r="188" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A188">
         <v>187</v>
       </c>
@@ -11458,7 +11468,7 @@
         <v>174.69591896156371</v>
       </c>
     </row>
-    <row r="189" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A189">
         <v>188</v>
       </c>
@@ -11508,7 +11518,7 @@
         <v>68.937846832953142</v>
       </c>
     </row>
-    <row r="190" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A190">
         <v>189</v>
       </c>
@@ -11558,7 +11568,7 @@
         <v>68.937846832953142</v>
       </c>
     </row>
-    <row r="191" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A191">
         <v>190</v>
       </c>
@@ -11608,7 +11618,7 @@
         <v>39.594785592329082</v>
       </c>
     </row>
-    <row r="192" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A192">
         <v>191</v>
       </c>
@@ -11658,7 +11668,7 @@
         <v>56.058338956679705</v>
       </c>
     </row>
-    <row r="193" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A193">
         <v>192</v>
       </c>
@@ -11708,7 +11718,7 @@
         <v>58.31431514210275</v>
       </c>
     </row>
-    <row r="194" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A194">
         <v>193</v>
       </c>
@@ -11758,7 +11768,7 @@
         <v>138.14717853272754</v>
       </c>
     </row>
-    <row r="195" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A195">
         <v>194</v>
       </c>
@@ -11808,7 +11818,7 @@
         <v>67.366238622050744</v>
       </c>
     </row>
-    <row r="196" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A196">
         <v>195</v>
       </c>
@@ -11858,7 +11868,7 @@
         <v>87.852936574331423</v>
       </c>
     </row>
-    <row r="197" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A197">
         <v>196</v>
       </c>
@@ -11908,7 +11918,7 @@
         <v>167.01660491977677</v>
       </c>
     </row>
-    <row r="198" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A198">
         <v>197</v>
       </c>
@@ -11958,7 +11968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A199">
         <v>198</v>
       </c>
@@ -12008,7 +12018,7 @@
         <v>24.602608405115184</v>
       </c>
     </row>
-    <row r="200" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A200">
         <v>199</v>
       </c>
@@ -12058,7 +12068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A201">
         <v>200</v>
       </c>
@@ -12108,7 +12118,7 @@
         <v>157.29597707212156</v>
       </c>
     </row>
-    <row r="202" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A202">
         <v>201</v>
       </c>
@@ -12158,7 +12168,7 @@
         <v>57.082818138061462</v>
       </c>
     </row>
-    <row r="203" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A203">
         <v>202</v>
       </c>
@@ -12208,7 +12218,7 @@
         <v>57.082818138061462</v>
       </c>
     </row>
-    <row r="204" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A204">
         <v>203</v>
       </c>
@@ -12258,7 +12268,7 @@
         <v>41.302358154923283</v>
       </c>
     </row>
-    <row r="205" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A205">
         <v>204</v>
       </c>
@@ -12308,7 +12318,7 @@
         <v>123.4550372283435</v>
       </c>
     </row>
-    <row r="206" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A206">
         <v>205</v>
       </c>
@@ -12358,7 +12368,7 @@
         <v>30.139290059323223</v>
       </c>
     </row>
-    <row r="207" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A207">
         <v>206</v>
       </c>
@@ -12408,7 +12418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A208">
         <v>207</v>
       </c>
@@ -12458,7 +12468,7 @@
         <v>473.65607643406065</v>
       </c>
     </row>
-    <row r="209" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A209">
         <v>208</v>
       </c>
@@ -12508,7 +12518,7 @@
         <v>473.65607643406065</v>
       </c>
     </row>
-    <row r="210" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A210">
         <v>209</v>
       </c>
@@ -12558,7 +12568,7 @@
         <v>121.05989669869788</v>
       </c>
     </row>
-    <row r="211" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A211">
         <v>210</v>
       </c>
@@ -12608,7 +12618,7 @@
         <v>281.66485602098993</v>
       </c>
     </row>
-    <row r="212" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A212">
         <v>211</v>
       </c>
@@ -12658,7 +12668,7 @@
         <v>281.66485602098993</v>
       </c>
     </row>
-    <row r="213" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A213">
         <v>212</v>
       </c>
@@ -12708,7 +12718,7 @@
         <v>121.05989669869788</v>
       </c>
     </row>
-    <row r="214" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A214">
         <v>213</v>
       </c>
@@ -12758,7 +12768,7 @@
         <v>121.05989669869788</v>
       </c>
     </row>
-    <row r="215" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A215">
         <v>214</v>
       </c>
@@ -12808,7 +12818,7 @@
         <v>121.05989669869788</v>
       </c>
     </row>
-    <row r="216" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A216">
         <v>215</v>
       </c>
@@ -12858,7 +12868,7 @@
         <v>121.05989669869788</v>
       </c>
     </row>
-    <row r="217" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A217">
         <v>216</v>
       </c>
@@ -12908,7 +12918,7 @@
         <v>121.05989669869788</v>
       </c>
     </row>
-    <row r="218" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A218">
         <v>217</v>
       </c>
@@ -12958,7 +12968,7 @@
         <v>343.46497259189414</v>
       </c>
     </row>
-    <row r="219" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A219">
         <v>218</v>
       </c>
@@ -13008,7 +13018,7 @@
         <v>343.46497259189414</v>
       </c>
     </row>
-    <row r="220" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A220">
         <v>219</v>
       </c>
@@ -13058,7 +13068,7 @@
         <v>121.05989669869788</v>
       </c>
     </row>
-    <row r="221" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A221">
         <v>220</v>
       </c>
@@ -13108,7 +13118,7 @@
         <v>121.05989669869788</v>
       </c>
     </row>
-    <row r="222" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A222">
         <v>221</v>
       </c>
@@ -13158,7 +13168,7 @@
         <v>121.05989669869788</v>
       </c>
     </row>
-    <row r="223" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A223">
         <v>222</v>
       </c>
@@ -13208,7 +13218,7 @@
         <v>121.05989669869788</v>
       </c>
     </row>
-    <row r="224" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A224">
         <v>223</v>
       </c>
@@ -13258,7 +13268,7 @@
         <v>121.05989669869788</v>
       </c>
     </row>
-    <row r="225" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A225">
         <v>224</v>
       </c>
@@ -13308,7 +13318,7 @@
         <v>121.05989669869788</v>
       </c>
     </row>
-    <row r="226" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A226">
         <v>225</v>
       </c>
@@ -13358,7 +13368,7 @@
         <v>121.05989669869788</v>
       </c>
     </row>
-    <row r="227" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A227">
         <v>226</v>
       </c>
@@ -13408,7 +13418,7 @@
         <v>121.05989669869788</v>
       </c>
     </row>
-    <row r="228" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A228">
         <v>227</v>
       </c>
@@ -13458,7 +13468,7 @@
         <v>121.05989669869788</v>
       </c>
     </row>
-    <row r="229" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A229">
         <v>228</v>
       </c>
@@ -13508,7 +13518,7 @@
         <v>121.05989669869788</v>
       </c>
     </row>
-    <row r="230" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A230">
         <v>229</v>
       </c>
@@ -13558,7 +13568,7 @@
         <v>121.05989669869788</v>
       </c>
     </row>
-    <row r="231" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A231">
         <v>230</v>
       </c>
@@ -13608,7 +13618,7 @@
         <v>121.05989669869788</v>
       </c>
     </row>
-    <row r="232" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A232">
         <v>231</v>
       </c>
@@ -13658,7 +13668,7 @@
         <v>121.05989669869788</v>
       </c>
     </row>
-    <row r="233" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A233">
         <v>232</v>
       </c>
@@ -13708,7 +13718,7 @@
         <v>6.0580595385819587</v>
       </c>
     </row>
-    <row r="234" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A234">
         <v>233</v>
       </c>
@@ -13758,7 +13768,7 @@
         <v>6.0580595385819587</v>
       </c>
     </row>
-    <row r="235" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A235">
         <v>234</v>
       </c>
@@ -13808,7 +13818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A236">
         <v>235</v>
       </c>
@@ -13859,6 +13869,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated column headers for easier reference
</commit_message>
<xml_diff>
--- a/data_spring_2025.xlsx
+++ b/data_spring_2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekgibbs/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekgibbs/Library/Mobile Documents/com~apple~CloudDocs/School/CourseCast/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B177733A-4988-B249-A603-BE0C7AC58620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80BB3F4-D3C3-AA43-9633-A7D2CBFB0C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-2100" windowWidth="38400" windowHeight="21100" xr2:uid="{26079AD5-63BA-6C45-88C1-5844B765A22E}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="561">
   <si>
     <t>ACCT6130001</t>
   </si>
@@ -1607,30 +1607,12 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>Instructor #1</t>
-  </si>
-  <si>
-    <t>Course Quality</t>
-  </si>
-  <si>
-    <t>Instructor Quality</t>
-  </si>
-  <si>
-    <t>Difficulty</t>
-  </si>
-  <si>
-    <t>Work Required</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
     <t>ORLOFF</t>
   </si>
   <si>
-    <t>Instructor #2</t>
-  </si>
-  <si>
     <t>INDARTE</t>
   </si>
   <si>
@@ -1649,9 +1631,6 @@
     <t>ADUSUMALLI</t>
   </si>
   <si>
-    <t>Instructor #3</t>
-  </si>
-  <si>
     <t>PONGELUPPE</t>
   </si>
   <si>
@@ -1689,6 +1668,63 @@
   </si>
   <si>
     <t>HOSANGAR</t>
+  </si>
+  <si>
+    <t>overall_course_quality</t>
+  </si>
+  <si>
+    <t>overall_instructor_quality</t>
+  </si>
+  <si>
+    <t>overall_difficulty</t>
+  </si>
+  <si>
+    <t>overall_work_required</t>
+  </si>
+  <si>
+    <t>instructor_1</t>
+  </si>
+  <si>
+    <t>instructor_1_course_quality</t>
+  </si>
+  <si>
+    <t>instructor_1_quality</t>
+  </si>
+  <si>
+    <t>instructor_1_difficulty</t>
+  </si>
+  <si>
+    <t>instructor_1_work_required</t>
+  </si>
+  <si>
+    <t>instructor_2_course_quality</t>
+  </si>
+  <si>
+    <t>instructor_2</t>
+  </si>
+  <si>
+    <t>instructor_2_quality</t>
+  </si>
+  <si>
+    <t>instructor_2_difficulty</t>
+  </si>
+  <si>
+    <t>instructor_2_work_required</t>
+  </si>
+  <si>
+    <t>instructor_3</t>
+  </si>
+  <si>
+    <t>instructor_3_course_quality</t>
+  </si>
+  <si>
+    <t>instructor_3_quality</t>
+  </si>
+  <si>
+    <t>instructor_3_difficulty</t>
+  </si>
+  <si>
+    <t>instructor_3_work_required</t>
   </si>
 </sst>
 </file>
@@ -1696,8 +1732,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.0"/>
-    <numFmt numFmtId="172" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -1822,7 +1858,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1831,7 +1867,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2171,11 +2207,11 @@
   <dimension ref="A1:AI236"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="N180" sqref="N180"/>
+      <selection pane="bottomRight" activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2247,61 +2283,61 @@
         <v>520</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>522</v>
+        <v>542</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>523</v>
+        <v>543</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>524</v>
+        <v>544</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>525</v>
+        <v>545</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>521</v>
+        <v>546</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>522</v>
+        <v>547</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>523</v>
+        <v>548</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>524</v>
+        <v>549</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>525</v>
+        <v>550</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>528</v>
+        <v>552</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>522</v>
+        <v>551</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>523</v>
+        <v>553</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>524</v>
+        <v>554</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>525</v>
+        <v>555</v>
       </c>
       <c r="AE1" s="2" t="s">
-        <v>535</v>
+        <v>556</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>522</v>
+        <v>557</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>523</v>
+        <v>558</v>
       </c>
       <c r="AH1" s="2" t="s">
-        <v>524</v>
+        <v>559</v>
       </c>
       <c r="AI1" s="2" t="s">
-        <v>525</v>
+        <v>560</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">
@@ -2973,31 +3009,31 @@
         <v>1</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="R10" s="9" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="S10" s="9" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="T10" s="9" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="U10" s="10" t="s">
         <v>9</v>
       </c>
       <c r="V10" s="9" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W10" s="9" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X10" s="9" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y10" s="9" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Z10" s="9"/>
       <c r="AA10" s="9"/>
@@ -3604,7 +3640,7 @@
         <v>2.5</v>
       </c>
       <c r="U18" s="7" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="V18" s="7">
         <v>3.27</v>
@@ -3758,7 +3794,7 @@
         <v>2.6</v>
       </c>
       <c r="U20" s="7" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="V20" s="7">
         <v>2.38</v>
@@ -3850,7 +3886,7 @@
         <v>2.6</v>
       </c>
       <c r="U21" s="7" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="V21" s="7">
         <v>2.38</v>
@@ -3942,7 +3978,7 @@
         <v>2.6</v>
       </c>
       <c r="U22" s="7" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="V22" s="7">
         <v>2.38</v>
@@ -4034,7 +4070,7 @@
         <v>2.6</v>
       </c>
       <c r="U23" s="7" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="V23" s="7">
         <v>2.38</v>
@@ -4129,19 +4165,19 @@
         <v>52</v>
       </c>
       <c r="V24" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W24" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X24" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y24" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Z24" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
@@ -4209,19 +4245,19 @@
         <v>52</v>
       </c>
       <c r="V25" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W25" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X25" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y25" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Z25" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
@@ -4289,19 +4325,19 @@
         <v>56</v>
       </c>
       <c r="V26" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W26" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X26" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y26" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Z26" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
@@ -4369,19 +4405,19 @@
         <v>56</v>
       </c>
       <c r="V27" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W27" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X27" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y27" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Z27" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.2">
@@ -4449,19 +4485,19 @@
         <v>56</v>
       </c>
       <c r="V28" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W28" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X28" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y28" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Z28" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
@@ -4529,19 +4565,19 @@
         <v>56</v>
       </c>
       <c r="V29" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W29" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X29" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y29" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Z29" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.2">
@@ -5148,16 +5184,16 @@
         <v>75</v>
       </c>
       <c r="V37" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W37" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X37" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y37" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.2">
@@ -5453,34 +5489,34 @@
         <v>2.6</v>
       </c>
       <c r="U41" s="7" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="V41" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W41" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X41" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y41" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Z41" s="7" t="s">
         <v>151</v>
       </c>
       <c r="AA41" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="AB41" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="AC41" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="AD41" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.2">
@@ -6149,31 +6185,31 @@
         <v>25.566815144068318</v>
       </c>
       <c r="Q50" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="R50" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="S50" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="T50" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="U50" s="7" t="s">
         <v>108</v>
       </c>
       <c r="V50" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W50" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X50" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y50" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="51" spans="1:30" x14ac:dyDescent="0.2">
@@ -6238,7 +6274,7 @@
         <v>2</v>
       </c>
       <c r="U51" s="7" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="V51" s="7">
         <v>2.75</v>
@@ -6253,7 +6289,7 @@
         <v>1.96</v>
       </c>
       <c r="Z51" s="7" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="AA51" s="7">
         <v>2.62</v>
@@ -6484,7 +6520,7 @@
         <v>1.7</v>
       </c>
       <c r="U54" s="7" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="V54" s="7">
         <v>2.38</v>
@@ -6499,7 +6535,7 @@
         <v>1.65</v>
       </c>
       <c r="Z54" s="7" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="AA54" s="7">
         <v>2.4300000000000002</v>
@@ -8233,7 +8269,7 @@
         <v>2.5299999999999998</v>
       </c>
       <c r="Z76" s="7" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="AA76" s="7">
         <v>2.85</v>
@@ -8248,19 +8284,19 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="AE76" s="7" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="AF76" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="AG76" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="AH76" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="AI76" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="77" spans="1:35" x14ac:dyDescent="0.2">
@@ -8340,7 +8376,7 @@
         <v>2.5299999999999998</v>
       </c>
       <c r="Z77" s="7" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="AA77" s="7">
         <v>2.85</v>
@@ -8355,19 +8391,19 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="AE77" s="7" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="AF77" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="AG77" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="AH77" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="AI77" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="78" spans="1:35" x14ac:dyDescent="0.2">
@@ -8447,7 +8483,7 @@
         <v>2.5299999999999998</v>
       </c>
       <c r="Z78" s="7" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="AA78" s="7">
         <v>2.85</v>
@@ -8462,19 +8498,19 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="AE78" s="7" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="AF78" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="AG78" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="AH78" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="AI78" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="79" spans="1:35" x14ac:dyDescent="0.2">
@@ -8539,7 +8575,7 @@
         <v>2.4</v>
       </c>
       <c r="U79" s="7" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="V79" s="7">
         <v>2.86</v>
@@ -8554,7 +8590,7 @@
         <v>2.41</v>
       </c>
       <c r="Z79" s="7" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="AA79" s="7">
         <v>2.52</v>
@@ -8569,7 +8605,7 @@
         <v>2.21</v>
       </c>
       <c r="AE79" s="7" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="AF79" s="7">
         <v>2.59</v>
@@ -8646,7 +8682,7 @@
         <v>2.4</v>
       </c>
       <c r="U80" s="7" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="V80" s="7">
         <v>2.86</v>
@@ -8661,7 +8697,7 @@
         <v>2.41</v>
       </c>
       <c r="Z80" s="7" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="AA80" s="7">
         <v>2.52</v>
@@ -8676,7 +8712,7 @@
         <v>2.21</v>
       </c>
       <c r="AE80" s="7" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="AF80" s="7">
         <v>2.59</v>
@@ -8753,7 +8789,7 @@
         <v>2.4</v>
       </c>
       <c r="U81" s="7" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="V81" s="7">
         <v>2.86</v>
@@ -8768,7 +8804,7 @@
         <v>2.41</v>
       </c>
       <c r="Z81" s="7" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="AA81" s="7">
         <v>2.52</v>
@@ -8783,7 +8819,7 @@
         <v>2.21</v>
       </c>
       <c r="AE81" s="7" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="AF81" s="7">
         <v>2.59</v>
@@ -9017,16 +9053,16 @@
         <v>189</v>
       </c>
       <c r="V84" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W84" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X84" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y84" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="85" spans="1:35" x14ac:dyDescent="0.2">
@@ -9091,7 +9127,7 @@
         <v>2</v>
       </c>
       <c r="U85" s="7" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="V85" s="7">
         <v>3.28</v>
@@ -9168,7 +9204,7 @@
         <v>2</v>
       </c>
       <c r="U86" s="7" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="V86" s="7">
         <v>3.28</v>
@@ -9849,31 +9885,31 @@
         <v>1</v>
       </c>
       <c r="Q95" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="R95" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="S95" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="T95" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="U95" s="7" t="s">
         <v>210</v>
       </c>
       <c r="V95" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W95" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X95" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y95" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="96" spans="1:35" x14ac:dyDescent="0.2">
@@ -10465,31 +10501,31 @@
         <v>1</v>
       </c>
       <c r="Q103" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="R103" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="S103" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="T103" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="U103" s="7" t="s">
         <v>229</v>
       </c>
       <c r="V103" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W103" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X103" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y103" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="104" spans="1:25" x14ac:dyDescent="0.2">
@@ -10773,31 +10809,31 @@
         <v>1101.0993426578223</v>
       </c>
       <c r="Q107" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="R107" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="S107" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="T107" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="U107" s="7" t="s">
         <v>239</v>
       </c>
       <c r="V107" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W107" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X107" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y107" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="108" spans="1:25" x14ac:dyDescent="0.2">
@@ -11555,7 +11591,7 @@
         <v>2.7</v>
       </c>
       <c r="U117" s="7" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="V117" s="7">
         <v>3.62</v>
@@ -11570,7 +11606,7 @@
         <v>2.67</v>
       </c>
       <c r="Z117" s="7" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="AA117" s="7">
         <v>3.62</v>
@@ -11727,16 +11763,16 @@
         <v>244</v>
       </c>
       <c r="V119" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W119" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X119" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y119" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="120" spans="1:30" x14ac:dyDescent="0.2">
@@ -12956,7 +12992,7 @@
         <v>1.8</v>
       </c>
       <c r="U135" s="7" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="V135" s="7">
         <v>2.82</v>
@@ -12971,7 +13007,7 @@
         <v>1.8</v>
       </c>
       <c r="Z135" s="7" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="AA135" s="7">
         <v>2.82</v>
@@ -14283,16 +14319,16 @@
         <v>333</v>
       </c>
       <c r="V152" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W152" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X152" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y152" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="153" spans="1:30" x14ac:dyDescent="0.2">
@@ -14434,7 +14470,7 @@
         <v>2.5</v>
       </c>
       <c r="U154" s="7" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="V154" s="7">
         <v>2.78</v>
@@ -14526,7 +14562,7 @@
         <v>2.5</v>
       </c>
       <c r="U155" s="7" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="V155" s="7">
         <v>2.78</v>
@@ -14618,7 +14654,7 @@
         <v>2.5</v>
       </c>
       <c r="U156" s="7" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="V156" s="7">
         <v>2.78</v>
@@ -15018,7 +15054,7 @@
         <v>2.5</v>
       </c>
       <c r="U161" s="7" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="V161" s="7">
         <v>2.99</v>
@@ -15172,7 +15208,7 @@
         <v>2.5</v>
       </c>
       <c r="U163" s="7" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="V163" s="7">
         <v>2.99</v>
@@ -15326,7 +15362,7 @@
         <v>2.5</v>
       </c>
       <c r="U165" s="7" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="V165" s="7">
         <v>2.99</v>
@@ -15480,7 +15516,7 @@
         <v>2.5</v>
       </c>
       <c r="U167" s="7" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="V167" s="7">
         <v>2.99</v>
@@ -16019,7 +16055,7 @@
         <v>1.7</v>
       </c>
       <c r="U174" s="7" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="V174" s="7">
         <v>3.03</v>
@@ -16099,16 +16135,16 @@
         <v>377</v>
       </c>
       <c r="V175" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W175" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X175" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y175" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="176" spans="1:25" x14ac:dyDescent="0.2">
@@ -16638,16 +16674,16 @@
         <v>390</v>
       </c>
       <c r="V182" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W182" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X182" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y182" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="183" spans="1:25" x14ac:dyDescent="0.2">
@@ -16715,16 +16751,16 @@
         <v>390</v>
       </c>
       <c r="V183" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W183" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X183" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y183" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="184" spans="1:25" x14ac:dyDescent="0.2">
@@ -16792,16 +16828,16 @@
         <v>390</v>
       </c>
       <c r="V184" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W184" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X184" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y184" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="185" spans="1:25" x14ac:dyDescent="0.2">
@@ -18009,31 +18045,31 @@
         <v>1</v>
       </c>
       <c r="Q200" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="R200" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="S200" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="T200" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="U200" s="7" t="s">
         <v>413</v>
       </c>
       <c r="V200" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W200" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X200" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y200" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="201" spans="1:25" x14ac:dyDescent="0.2">
@@ -18101,16 +18137,16 @@
         <v>432</v>
       </c>
       <c r="V201" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W201" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X201" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y201" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="202" spans="1:25" x14ac:dyDescent="0.2">
@@ -18178,16 +18214,16 @@
         <v>432</v>
       </c>
       <c r="V202" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W202" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X202" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y202" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="203" spans="1:25" x14ac:dyDescent="0.2">
@@ -18255,16 +18291,16 @@
         <v>432</v>
       </c>
       <c r="V203" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W203" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X203" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y203" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="204" spans="1:25" x14ac:dyDescent="0.2">
@@ -18409,16 +18445,16 @@
         <v>441</v>
       </c>
       <c r="V205" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W205" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X205" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y205" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="206" spans="1:25" x14ac:dyDescent="0.2">
@@ -18548,31 +18584,31 @@
         <v>1</v>
       </c>
       <c r="Q207" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="R207" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="S207" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="T207" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="U207" s="7" t="s">
         <v>447</v>
       </c>
       <c r="V207" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W207" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X207" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y207" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="208" spans="1:25" x14ac:dyDescent="0.2">
@@ -18794,16 +18830,16 @@
         <v>454</v>
       </c>
       <c r="V210" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W210" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X210" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y210" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="211" spans="1:25" x14ac:dyDescent="0.2">
@@ -18871,16 +18907,16 @@
         <v>456</v>
       </c>
       <c r="V211" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W211" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X211" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y211" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="212" spans="1:25" x14ac:dyDescent="0.2">
@@ -18948,16 +18984,16 @@
         <v>456</v>
       </c>
       <c r="V212" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W212" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X212" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y212" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="213" spans="1:25" x14ac:dyDescent="0.2">
@@ -19025,16 +19061,16 @@
         <v>459</v>
       </c>
       <c r="V213" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W213" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X213" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y213" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="214" spans="1:25" x14ac:dyDescent="0.2">
@@ -19102,16 +19138,16 @@
         <v>461</v>
       </c>
       <c r="V214" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W214" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X214" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y214" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="215" spans="1:25" x14ac:dyDescent="0.2">
@@ -19179,16 +19215,16 @@
         <v>463</v>
       </c>
       <c r="V215" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W215" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X215" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y215" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="216" spans="1:25" x14ac:dyDescent="0.2">
@@ -19256,16 +19292,16 @@
         <v>465</v>
       </c>
       <c r="V216" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W216" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X216" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y216" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="217" spans="1:25" x14ac:dyDescent="0.2">
@@ -19333,16 +19369,16 @@
         <v>467</v>
       </c>
       <c r="V217" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W217" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X217" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y217" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="218" spans="1:25" x14ac:dyDescent="0.2">
@@ -19410,16 +19446,16 @@
         <v>469</v>
       </c>
       <c r="V218" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W218" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X218" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y218" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="219" spans="1:25" x14ac:dyDescent="0.2">
@@ -19487,16 +19523,16 @@
         <v>469</v>
       </c>
       <c r="V219" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W219" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X219" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y219" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="220" spans="1:25" x14ac:dyDescent="0.2">
@@ -19564,16 +19600,16 @@
         <v>472</v>
       </c>
       <c r="V220" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W220" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X220" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y220" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="221" spans="1:25" x14ac:dyDescent="0.2">
@@ -19641,16 +19677,16 @@
         <v>474</v>
       </c>
       <c r="V221" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W221" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X221" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y221" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="222" spans="1:25" x14ac:dyDescent="0.2">
@@ -19718,16 +19754,16 @@
         <v>476</v>
       </c>
       <c r="V222" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W222" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X222" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y222" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="223" spans="1:25" x14ac:dyDescent="0.2">
@@ -19795,16 +19831,16 @@
         <v>478</v>
       </c>
       <c r="V223" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W223" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X223" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y223" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="224" spans="1:25" x14ac:dyDescent="0.2">
@@ -19872,16 +19908,16 @@
         <v>480</v>
       </c>
       <c r="V224" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W224" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X224" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y224" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="225" spans="1:25" x14ac:dyDescent="0.2">
@@ -19949,16 +19985,16 @@
         <v>482</v>
       </c>
       <c r="V225" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W225" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X225" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y225" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="226" spans="1:25" x14ac:dyDescent="0.2">
@@ -20026,16 +20062,16 @@
         <v>484</v>
       </c>
       <c r="V226" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W226" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X226" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y226" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="227" spans="1:25" x14ac:dyDescent="0.2">
@@ -20103,16 +20139,16 @@
         <v>486</v>
       </c>
       <c r="V227" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W227" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X227" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y227" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="228" spans="1:25" x14ac:dyDescent="0.2">
@@ -20180,16 +20216,16 @@
         <v>488</v>
       </c>
       <c r="V228" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W228" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X228" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y228" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="229" spans="1:25" x14ac:dyDescent="0.2">
@@ -20257,16 +20293,16 @@
         <v>490</v>
       </c>
       <c r="V229" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W229" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X229" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y229" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="230" spans="1:25" x14ac:dyDescent="0.2">
@@ -20334,16 +20370,16 @@
         <v>492</v>
       </c>
       <c r="V230" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W230" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X230" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y230" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="231" spans="1:25" x14ac:dyDescent="0.2">
@@ -20411,16 +20447,16 @@
         <v>494</v>
       </c>
       <c r="V231" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W231" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X231" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y231" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="232" spans="1:25" x14ac:dyDescent="0.2">
@@ -20488,16 +20524,16 @@
         <v>478</v>
       </c>
       <c r="V232" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W232" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X232" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y232" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="233" spans="1:25" x14ac:dyDescent="0.2">
@@ -20642,16 +20678,16 @@
         <v>500</v>
       </c>
       <c r="V234" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="W234" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="X234" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Y234" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="235" spans="1:25" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added course eval data
</commit_message>
<xml_diff>
--- a/data_spring_2025.xlsx
+++ b/data_spring_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekgibbs/Library/Mobile Documents/com~apple~CloudDocs/School/CourseCast/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80BB3F4-D3C3-AA43-9633-A7D2CBFB0C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E3A5C9-2D5C-C84E-8895-7F01EF299B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-2100" windowWidth="38400" windowHeight="21100" xr2:uid="{26079AD5-63BA-6C45-88C1-5844B765A22E}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$B$1:$N$236</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$C$1:$AI$236</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="560">
   <si>
     <t>ACCT6130001</t>
   </si>
@@ -1605,9 +1605,6 @@
   <si>
     <t>resid_stdev</t>
     <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>ORLOFF</t>
@@ -2207,11 +2204,11 @@
   <dimension ref="A1:AI236"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="AI2" sqref="AI2"/>
+      <selection pane="bottomRight" activeCell="AM77" sqref="AM77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2226,11 +2223,7 @@
     <col min="18" max="18" width="14.83203125" style="7" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.6640625" style="7"/>
-    <col min="22" max="22" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.83203125" style="7" customWidth="1"/>
-    <col min="24" max="24" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="35" width="10.6640625" style="7"/>
+    <col min="21" max="35" width="14.83203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
@@ -2283,61 +2276,61 @@
         <v>520</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="AA1" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="AA1" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>559</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">
@@ -3008,33 +3001,17 @@
       <c r="P10" s="6">
         <v>1</v>
       </c>
-      <c r="Q10" s="9" t="s">
-        <v>521</v>
-      </c>
-      <c r="R10" s="9" t="s">
-        <v>521</v>
-      </c>
-      <c r="S10" s="9" t="s">
-        <v>521</v>
-      </c>
-      <c r="T10" s="9" t="s">
-        <v>521</v>
-      </c>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
       <c r="U10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="V10" s="9" t="s">
-        <v>521</v>
-      </c>
-      <c r="W10" s="9" t="s">
-        <v>521</v>
-      </c>
-      <c r="X10" s="9" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y10" s="9" t="s">
-        <v>521</v>
-      </c>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
       <c r="Z10" s="9"/>
       <c r="AA10" s="9"/>
       <c r="AB10" s="9"/>
@@ -3640,7 +3617,7 @@
         <v>2.5</v>
       </c>
       <c r="U18" s="7" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="V18" s="7">
         <v>3.27</v>
@@ -3794,7 +3771,7 @@
         <v>2.6</v>
       </c>
       <c r="U20" s="7" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="V20" s="7">
         <v>2.38</v>
@@ -3886,7 +3863,7 @@
         <v>2.6</v>
       </c>
       <c r="U21" s="7" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="V21" s="7">
         <v>2.38</v>
@@ -3978,7 +3955,7 @@
         <v>2.6</v>
       </c>
       <c r="U22" s="7" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="V22" s="7">
         <v>2.38</v>
@@ -4070,7 +4047,7 @@
         <v>2.6</v>
       </c>
       <c r="U23" s="7" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="V23" s="7">
         <v>2.38</v>
@@ -4164,21 +4141,6 @@
       <c r="U24" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="V24" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W24" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X24" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y24" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Z24" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25">
@@ -4244,21 +4206,6 @@
       <c r="U25" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="V25" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W25" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X25" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y25" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Z25" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26">
@@ -4324,21 +4271,6 @@
       <c r="U26" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="V26" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W26" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X26" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y26" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Z26" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -4404,21 +4336,6 @@
       <c r="U27" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="V27" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W27" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X27" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y27" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Z27" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28">
@@ -4484,21 +4401,6 @@
       <c r="U28" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="V28" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W28" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X28" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y28" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Z28" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29">
@@ -4564,21 +4466,6 @@
       <c r="U29" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="V29" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W29" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X29" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y29" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Z29" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30">
@@ -4811,7 +4698,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4888,7 +4775,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4965,7 +4852,7 @@
         <v>3.48</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5042,7 +4929,7 @@
         <v>3.48</v>
       </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5119,7 +5006,7 @@
         <v>2.33</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5183,20 +5070,8 @@
       <c r="U37" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="V37" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W37" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X37" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y37" s="7" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5273,7 +5148,7 @@
         <v>2.89</v>
       </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5350,7 +5225,7 @@
         <v>3.08</v>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5427,7 +5302,7 @@
         <v>3.08</v>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5489,37 +5364,13 @@
         <v>2.6</v>
       </c>
       <c r="U41" s="7" t="s">
-        <v>524</v>
-      </c>
-      <c r="V41" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W41" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X41" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y41" s="7" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="Z41" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="AA41" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="AB41" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="AC41" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="AD41" s="7" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5596,7 +5447,7 @@
         <v>2.4700000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5673,7 +5524,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5750,7 +5601,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5827,7 +5678,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5904,7 +5755,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5981,7 +5832,7 @@
         <v>2.13</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -6184,32 +6035,8 @@
       <c r="P50" s="6">
         <v>25.566815144068318</v>
       </c>
-      <c r="Q50" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="R50" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="S50" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="T50" s="7" t="s">
-        <v>521</v>
-      </c>
       <c r="U50" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="V50" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W50" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X50" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y50" s="7" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="51" spans="1:30" x14ac:dyDescent="0.2">
@@ -6274,7 +6101,7 @@
         <v>2</v>
       </c>
       <c r="U51" s="7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="V51" s="7">
         <v>2.75</v>
@@ -6289,7 +6116,7 @@
         <v>1.96</v>
       </c>
       <c r="Z51" s="7" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="AA51" s="7">
         <v>2.62</v>
@@ -6520,7 +6347,7 @@
         <v>1.7</v>
       </c>
       <c r="U54" s="7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="V54" s="7">
         <v>2.38</v>
@@ -6535,7 +6362,7 @@
         <v>1.65</v>
       </c>
       <c r="Z54" s="7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="AA54" s="7">
         <v>2.4300000000000002</v>
@@ -8269,7 +8096,7 @@
         <v>2.5299999999999998</v>
       </c>
       <c r="Z76" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="AA76" s="7">
         <v>2.85</v>
@@ -8284,19 +8111,7 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="AE76" s="7" t="s">
-        <v>530</v>
-      </c>
-      <c r="AF76" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="AG76" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="AH76" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="AI76" s="7" t="s">
-        <v>521</v>
+        <v>529</v>
       </c>
     </row>
     <row r="77" spans="1:35" x14ac:dyDescent="0.2">
@@ -8376,7 +8191,7 @@
         <v>2.5299999999999998</v>
       </c>
       <c r="Z77" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="AA77" s="7">
         <v>2.85</v>
@@ -8391,19 +8206,7 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="AE77" s="7" t="s">
-        <v>530</v>
-      </c>
-      <c r="AF77" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="AG77" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="AH77" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="AI77" s="7" t="s">
-        <v>521</v>
+        <v>529</v>
       </c>
     </row>
     <row r="78" spans="1:35" x14ac:dyDescent="0.2">
@@ -8483,7 +8286,7 @@
         <v>2.5299999999999998</v>
       </c>
       <c r="Z78" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="AA78" s="7">
         <v>2.85</v>
@@ -8498,19 +8301,7 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="AE78" s="7" t="s">
-        <v>530</v>
-      </c>
-      <c r="AF78" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="AG78" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="AH78" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="AI78" s="7" t="s">
-        <v>521</v>
+        <v>529</v>
       </c>
     </row>
     <row r="79" spans="1:35" x14ac:dyDescent="0.2">
@@ -8575,7 +8366,7 @@
         <v>2.4</v>
       </c>
       <c r="U79" s="7" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="V79" s="7">
         <v>2.86</v>
@@ -8590,7 +8381,7 @@
         <v>2.41</v>
       </c>
       <c r="Z79" s="7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AA79" s="7">
         <v>2.52</v>
@@ -8605,7 +8396,7 @@
         <v>2.21</v>
       </c>
       <c r="AE79" s="7" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AF79" s="7">
         <v>2.59</v>
@@ -8682,7 +8473,7 @@
         <v>2.4</v>
       </c>
       <c r="U80" s="7" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="V80" s="7">
         <v>2.86</v>
@@ -8697,7 +8488,7 @@
         <v>2.41</v>
       </c>
       <c r="Z80" s="7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AA80" s="7">
         <v>2.52</v>
@@ -8712,7 +8503,7 @@
         <v>2.21</v>
       </c>
       <c r="AE80" s="7" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AF80" s="7">
         <v>2.59</v>
@@ -8789,7 +8580,7 @@
         <v>2.4</v>
       </c>
       <c r="U81" s="7" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="V81" s="7">
         <v>2.86</v>
@@ -8804,7 +8595,7 @@
         <v>2.41</v>
       </c>
       <c r="Z81" s="7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AA81" s="7">
         <v>2.52</v>
@@ -8819,7 +8610,7 @@
         <v>2.21</v>
       </c>
       <c r="AE81" s="7" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AF81" s="7">
         <v>2.59</v>
@@ -9052,18 +8843,6 @@
       <c r="U84" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="V84" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W84" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X84" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y84" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="85" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A85">
@@ -9127,7 +8906,7 @@
         <v>2</v>
       </c>
       <c r="U85" s="7" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="V85" s="7">
         <v>3.28</v>
@@ -9204,7 +8983,7 @@
         <v>2</v>
       </c>
       <c r="U86" s="7" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="V86" s="7">
         <v>3.28</v>
@@ -9884,32 +9663,8 @@
       <c r="P95" s="6">
         <v>1</v>
       </c>
-      <c r="Q95" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="R95" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="S95" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="T95" s="7" t="s">
-        <v>521</v>
-      </c>
       <c r="U95" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="V95" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W95" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X95" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y95" s="7" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="96" spans="1:35" x14ac:dyDescent="0.2">
@@ -10500,32 +10255,8 @@
       <c r="P103" s="6">
         <v>1</v>
       </c>
-      <c r="Q103" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="R103" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="S103" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="T103" s="7" t="s">
-        <v>521</v>
-      </c>
       <c r="U103" s="7" t="s">
         <v>229</v>
-      </c>
-      <c r="V103" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W103" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X103" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y103" s="7" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="104" spans="1:25" x14ac:dyDescent="0.2">
@@ -10808,32 +10539,8 @@
       <c r="P107" s="6">
         <v>1101.0993426578223</v>
       </c>
-      <c r="Q107" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="R107" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="S107" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="T107" s="7" t="s">
-        <v>521</v>
-      </c>
       <c r="U107" s="7" t="s">
         <v>239</v>
-      </c>
-      <c r="V107" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W107" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X107" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y107" s="7" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="108" spans="1:25" x14ac:dyDescent="0.2">
@@ -11591,7 +11298,7 @@
         <v>2.7</v>
       </c>
       <c r="U117" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="V117" s="7">
         <v>3.62</v>
@@ -11606,7 +11313,7 @@
         <v>2.67</v>
       </c>
       <c r="Z117" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="AA117" s="7">
         <v>3.62</v>
@@ -11762,18 +11469,6 @@
       <c r="U119" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="V119" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W119" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X119" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y119" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="120" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A120">
@@ -12992,7 +12687,7 @@
         <v>1.8</v>
       </c>
       <c r="U135" s="7" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="V135" s="7">
         <v>2.82</v>
@@ -13007,7 +12702,7 @@
         <v>1.8</v>
       </c>
       <c r="Z135" s="7" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AA135" s="7">
         <v>2.82</v>
@@ -14318,18 +14013,6 @@
       <c r="U152" s="7" t="s">
         <v>333</v>
       </c>
-      <c r="V152" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W152" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X152" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y152" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="153" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A153">
@@ -14470,7 +14153,7 @@
         <v>2.5</v>
       </c>
       <c r="U154" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="V154" s="7">
         <v>2.78</v>
@@ -14562,7 +14245,7 @@
         <v>2.5</v>
       </c>
       <c r="U155" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="V155" s="7">
         <v>2.78</v>
@@ -14654,7 +14337,7 @@
         <v>2.5</v>
       </c>
       <c r="U156" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="V156" s="7">
         <v>2.78</v>
@@ -15054,7 +14737,7 @@
         <v>2.5</v>
       </c>
       <c r="U161" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="V161" s="7">
         <v>2.99</v>
@@ -15208,7 +14891,7 @@
         <v>2.5</v>
       </c>
       <c r="U163" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="V163" s="7">
         <v>2.99</v>
@@ -15362,7 +15045,7 @@
         <v>2.5</v>
       </c>
       <c r="U165" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="V165" s="7">
         <v>2.99</v>
@@ -15516,7 +15199,7 @@
         <v>2.5</v>
       </c>
       <c r="U167" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="V167" s="7">
         <v>2.99</v>
@@ -16055,7 +15738,7 @@
         <v>1.7</v>
       </c>
       <c r="U174" s="7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="V174" s="7">
         <v>3.03</v>
@@ -16134,18 +15817,6 @@
       <c r="U175" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="V175" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W175" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X175" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y175" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="176" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A176">
@@ -16673,18 +16344,6 @@
       <c r="U182" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="V182" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W182" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X182" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y182" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="183" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A183">
@@ -16750,18 +16409,6 @@
       <c r="U183" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="V183" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W183" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X183" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y183" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="184" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A184">
@@ -16827,18 +16474,6 @@
       <c r="U184" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="V184" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W184" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X184" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y184" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="185" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A185">
@@ -18044,32 +17679,8 @@
       <c r="P200" s="6">
         <v>1</v>
       </c>
-      <c r="Q200" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="R200" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="S200" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="T200" s="7" t="s">
-        <v>521</v>
-      </c>
       <c r="U200" s="7" t="s">
         <v>413</v>
-      </c>
-      <c r="V200" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W200" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X200" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y200" s="7" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="201" spans="1:25" x14ac:dyDescent="0.2">
@@ -18136,18 +17747,6 @@
       <c r="U201" s="7" t="s">
         <v>432</v>
       </c>
-      <c r="V201" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W201" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X201" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y201" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="202" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A202">
@@ -18213,18 +17812,6 @@
       <c r="U202" s="7" t="s">
         <v>432</v>
       </c>
-      <c r="V202" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W202" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X202" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y202" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="203" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A203">
@@ -18290,18 +17877,6 @@
       <c r="U203" s="7" t="s">
         <v>432</v>
       </c>
-      <c r="V203" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W203" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X203" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y203" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="204" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A204">
@@ -18444,18 +18019,6 @@
       <c r="U205" s="7" t="s">
         <v>441</v>
       </c>
-      <c r="V205" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W205" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X205" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y205" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="206" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A206">
@@ -18583,32 +18146,8 @@
       <c r="P207" s="6">
         <v>1</v>
       </c>
-      <c r="Q207" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="R207" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="S207" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="T207" s="7" t="s">
-        <v>521</v>
-      </c>
       <c r="U207" s="7" t="s">
         <v>447</v>
-      </c>
-      <c r="V207" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W207" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X207" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y207" s="7" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="208" spans="1:25" x14ac:dyDescent="0.2">
@@ -18829,18 +18368,6 @@
       <c r="U210" s="7" t="s">
         <v>454</v>
       </c>
-      <c r="V210" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W210" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X210" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y210" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="211" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A211">
@@ -18906,18 +18433,6 @@
       <c r="U211" s="7" t="s">
         <v>456</v>
       </c>
-      <c r="V211" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W211" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X211" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y211" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="212" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A212">
@@ -18983,18 +18498,6 @@
       <c r="U212" s="7" t="s">
         <v>456</v>
       </c>
-      <c r="V212" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W212" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X212" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y212" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="213" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A213">
@@ -19060,18 +18563,6 @@
       <c r="U213" s="7" t="s">
         <v>459</v>
       </c>
-      <c r="V213" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W213" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X213" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y213" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="214" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A214">
@@ -19137,18 +18628,6 @@
       <c r="U214" s="7" t="s">
         <v>461</v>
       </c>
-      <c r="V214" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W214" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X214" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y214" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="215" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A215">
@@ -19214,18 +18693,6 @@
       <c r="U215" s="7" t="s">
         <v>463</v>
       </c>
-      <c r="V215" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W215" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X215" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y215" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="216" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A216">
@@ -19291,18 +18758,6 @@
       <c r="U216" s="7" t="s">
         <v>465</v>
       </c>
-      <c r="V216" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W216" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X216" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y216" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="217" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A217">
@@ -19368,18 +18823,6 @@
       <c r="U217" s="7" t="s">
         <v>467</v>
       </c>
-      <c r="V217" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W217" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X217" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y217" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="218" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A218">
@@ -19445,18 +18888,6 @@
       <c r="U218" s="7" t="s">
         <v>469</v>
       </c>
-      <c r="V218" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W218" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X218" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y218" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="219" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A219">
@@ -19522,18 +18953,6 @@
       <c r="U219" s="7" t="s">
         <v>469</v>
       </c>
-      <c r="V219" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W219" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X219" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y219" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="220" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A220">
@@ -19599,18 +19018,6 @@
       <c r="U220" s="7" t="s">
         <v>472</v>
       </c>
-      <c r="V220" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W220" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X220" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y220" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="221" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A221">
@@ -19676,18 +19083,6 @@
       <c r="U221" s="7" t="s">
         <v>474</v>
       </c>
-      <c r="V221" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W221" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X221" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y221" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="222" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A222">
@@ -19753,18 +19148,6 @@
       <c r="U222" s="7" t="s">
         <v>476</v>
       </c>
-      <c r="V222" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W222" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X222" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y222" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="223" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A223">
@@ -19830,18 +19213,6 @@
       <c r="U223" s="7" t="s">
         <v>478</v>
       </c>
-      <c r="V223" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W223" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X223" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y223" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="224" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A224">
@@ -19907,18 +19278,6 @@
       <c r="U224" s="7" t="s">
         <v>480</v>
       </c>
-      <c r="V224" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W224" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X224" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y224" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="225" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A225">
@@ -19984,18 +19343,6 @@
       <c r="U225" s="7" t="s">
         <v>482</v>
       </c>
-      <c r="V225" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W225" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X225" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y225" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="226" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A226">
@@ -20061,18 +19408,6 @@
       <c r="U226" s="7" t="s">
         <v>484</v>
       </c>
-      <c r="V226" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W226" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X226" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y226" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="227" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A227">
@@ -20138,18 +19473,6 @@
       <c r="U227" s="7" t="s">
         <v>486</v>
       </c>
-      <c r="V227" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W227" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X227" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y227" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="228" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A228">
@@ -20215,18 +19538,6 @@
       <c r="U228" s="7" t="s">
         <v>488</v>
       </c>
-      <c r="V228" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W228" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X228" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y228" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="229" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A229">
@@ -20292,18 +19603,6 @@
       <c r="U229" s="7" t="s">
         <v>490</v>
       </c>
-      <c r="V229" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W229" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X229" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y229" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="230" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A230">
@@ -20369,18 +19668,6 @@
       <c r="U230" s="7" t="s">
         <v>492</v>
       </c>
-      <c r="V230" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W230" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X230" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y230" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="231" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A231">
@@ -20446,18 +19733,6 @@
       <c r="U231" s="7" t="s">
         <v>494</v>
       </c>
-      <c r="V231" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W231" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X231" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y231" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="232" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A232">
@@ -20523,18 +19798,6 @@
       <c r="U232" s="7" t="s">
         <v>478</v>
       </c>
-      <c r="V232" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W232" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X232" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y232" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="233" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A233">
@@ -20677,18 +19940,6 @@
       <c r="U234" s="7" t="s">
         <v>500</v>
       </c>
-      <c r="V234" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="W234" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="X234" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="Y234" s="7" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="235" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A235">
@@ -20845,6 +20096,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="C1:AI236" xr:uid="{A458C66A-1996-8645-A24F-CDFC1D0B0EC5}"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
fixed 1:30pm class time and Exec Leadership CU
</commit_message>
<xml_diff>
--- a/data_spring_2025.xlsx
+++ b/data_spring_2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekgibbs/Library/Mobile Documents/com~apple~CloudDocs/School/CourseCast/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekgibbs/Documents/Projects/CourseCast/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E3A5C9-2D5C-C84E-8895-7F01EF299B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF95CD10-7181-BE49-AF15-3FAEA9159E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-2100" windowWidth="38400" windowHeight="21100" xr2:uid="{26079AD5-63BA-6C45-88C1-5844B765A22E}"/>
   </bookViews>
@@ -2204,11 +2204,11 @@
   <dimension ref="A1:AI236"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F47" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="AM77" sqref="AM77"/>
+      <selection pane="bottomRight" activeCell="L85" sqref="L85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6015,7 +6015,7 @@
         <v>105</v>
       </c>
       <c r="J50" s="11">
-        <v>0.5625</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="K50" s="11">
         <v>0.64583333333333337</v>
@@ -8814,7 +8814,7 @@
         <v>0.48888888888888887</v>
       </c>
       <c r="L84">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M84">
         <v>72</v>

</xml_diff>

<commit_message>
fixed MDM, added WHCP, and updated min resid
</commit_message>
<xml_diff>
--- a/data_spring_2025.xlsx
+++ b/data_spring_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekgibbs/Documents/Projects/CourseCast/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF95CD10-7181-BE49-AF15-3FAEA9159E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE4FAAA-8D8B-894E-838C-9DF59DA24430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-2100" windowWidth="38400" windowHeight="21100" xr2:uid="{26079AD5-63BA-6C45-88C1-5844B765A22E}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$C$1:$AI$236</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$C$1:$AI$237</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="561">
   <si>
     <t>ACCT6130001</t>
   </si>
@@ -1722,6 +1722,9 @@
   </si>
   <si>
     <t>instructor_3_work_required</t>
+  </si>
+  <si>
+    <t>WHCP6180003</t>
   </si>
 </sst>
 </file>
@@ -1789,7 +1792,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1826,6 +1829,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1840,7 +1849,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1865,6 +1874,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2201,14 +2211,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A458C66A-1996-8645-A24F-CDFC1D0B0EC5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AI236"/>
+  <dimension ref="A1:AI237"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F69" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="L85" sqref="L85"/>
+      <selection pane="bottomRight" activeCell="J96" sqref="J96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2841,8 +2851,8 @@
       <c r="O8" s="6">
         <v>-0.38243792329610993</v>
       </c>
-      <c r="P8" s="6">
-        <v>0.66240191388999159</v>
+      <c r="P8" s="12">
+        <v>50</v>
       </c>
       <c r="Q8" s="7">
         <v>3.3</v>
@@ -2998,8 +3008,8 @@
       <c r="O10" s="6">
         <v>0</v>
       </c>
-      <c r="P10" s="6">
-        <v>1</v>
+      <c r="P10" s="12">
+        <v>50</v>
       </c>
       <c r="Q10" s="9"/>
       <c r="R10" s="9"/>
@@ -3062,8 +3072,8 @@
       <c r="O11" s="6">
         <v>0</v>
       </c>
-      <c r="P11" s="6">
-        <v>1</v>
+      <c r="P11" s="12">
+        <v>50</v>
       </c>
       <c r="Q11" s="7">
         <v>3.2</v>
@@ -3139,8 +3149,8 @@
       <c r="O12" s="6">
         <v>0</v>
       </c>
-      <c r="P12" s="6">
-        <v>1</v>
+      <c r="P12" s="12">
+        <v>50</v>
       </c>
       <c r="Q12" s="7">
         <v>3.2</v>
@@ -3524,8 +3534,8 @@
       <c r="O17" s="6">
         <v>0</v>
       </c>
-      <c r="P17" s="6">
-        <v>1</v>
+      <c r="P17" s="12">
+        <v>50</v>
       </c>
       <c r="Q17" s="7">
         <v>2.6</v>
@@ -6331,8 +6341,8 @@
       <c r="O54" s="6">
         <v>0</v>
       </c>
-      <c r="P54" s="6">
-        <v>0</v>
+      <c r="P54" s="12">
+        <v>25</v>
       </c>
       <c r="Q54" s="7">
         <v>2.2999999999999998</v>
@@ -6654,8 +6664,8 @@
       <c r="O58" s="6">
         <v>0</v>
       </c>
-      <c r="P58" s="6">
-        <v>0</v>
+      <c r="P58" s="12">
+        <v>50</v>
       </c>
       <c r="Q58" s="7">
         <v>2.6</v>
@@ -6731,8 +6741,8 @@
       <c r="O59" s="6">
         <v>0</v>
       </c>
-      <c r="P59" s="6">
-        <v>0</v>
+      <c r="P59" s="12">
+        <v>50</v>
       </c>
       <c r="Q59" s="7">
         <v>2.6</v>
@@ -7059,8 +7069,8 @@
       <c r="O63" s="6">
         <v>30.701795939522071</v>
       </c>
-      <c r="P63" s="6">
-        <v>0.27783475903992005</v>
+      <c r="P63" s="12">
+        <v>50</v>
       </c>
       <c r="Q63" s="7">
         <v>2.6</v>
@@ -7141,8 +7151,8 @@
       <c r="O64" s="6">
         <v>30.701795939522071</v>
       </c>
-      <c r="P64" s="6">
-        <v>0.27783475903992005</v>
+      <c r="P64" s="12">
+        <v>50</v>
       </c>
       <c r="Q64" s="7">
         <v>2.6</v>
@@ -9660,8 +9670,8 @@
       <c r="O95" s="6">
         <v>0</v>
       </c>
-      <c r="P95" s="6">
-        <v>1</v>
+      <c r="P95" s="12">
+        <v>50</v>
       </c>
       <c r="U95" s="7" t="s">
         <v>210</v>
@@ -10252,8 +10262,8 @@
       <c r="O103" s="6">
         <v>0</v>
       </c>
-      <c r="P103" s="6">
-        <v>1</v>
+      <c r="P103" s="12">
+        <v>50</v>
       </c>
       <c r="U103" s="7" t="s">
         <v>229</v>
@@ -12994,8 +13004,8 @@
       <c r="O139" s="6">
         <v>0</v>
       </c>
-      <c r="P139" s="6">
-        <v>1</v>
+      <c r="P139" s="12">
+        <v>50</v>
       </c>
       <c r="Q139" s="7">
         <v>2.2999999999999998</v>
@@ -13148,8 +13158,8 @@
       <c r="O141" s="6">
         <v>1.4794141641911573</v>
       </c>
-      <c r="P141" s="6">
-        <v>18.990840069725987</v>
+      <c r="P141" s="12">
+        <v>50</v>
       </c>
       <c r="Q141" s="7">
         <v>2.9</v>
@@ -13225,8 +13235,8 @@
       <c r="O142" s="6">
         <v>0</v>
       </c>
-      <c r="P142" s="6">
-        <v>0</v>
+      <c r="P142" s="12">
+        <v>25</v>
       </c>
       <c r="Q142" s="7">
         <v>2.9</v>
@@ -13302,8 +13312,8 @@
       <c r="O143" s="6">
         <v>0</v>
       </c>
-      <c r="P143" s="6">
-        <v>1</v>
+      <c r="P143" s="12">
+        <v>50</v>
       </c>
       <c r="Q143" s="7">
         <v>2.5</v>
@@ -13379,8 +13389,8 @@
       <c r="O144" s="6">
         <v>0</v>
       </c>
-      <c r="P144" s="6">
-        <v>1</v>
+      <c r="P144" s="12">
+        <v>50</v>
       </c>
       <c r="Q144" s="7">
         <v>2.5</v>
@@ -13764,8 +13774,8 @@
       <c r="O149" s="6">
         <v>0</v>
       </c>
-      <c r="P149" s="6">
-        <v>0</v>
+      <c r="P149" s="12">
+        <v>50</v>
       </c>
       <c r="Q149" s="7">
         <v>3.3</v>
@@ -13841,8 +13851,8 @@
       <c r="O150" s="6">
         <v>0</v>
       </c>
-      <c r="P150" s="6">
-        <v>0</v>
+      <c r="P150" s="12">
+        <v>50</v>
       </c>
       <c r="Q150" s="7">
         <v>3.3</v>
@@ -13995,8 +14005,8 @@
       <c r="O152" s="6">
         <v>0</v>
       </c>
-      <c r="P152" s="6">
-        <v>1</v>
+      <c r="P152" s="12">
+        <v>50</v>
       </c>
       <c r="Q152" s="7">
         <v>2.4</v>
@@ -15723,7 +15733,7 @@
         <v>-96.226257446766439</v>
       </c>
       <c r="P174" s="6">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="Q174" s="7">
         <v>3</v>
@@ -15800,7 +15810,7 @@
         <v>-96.226257446766439</v>
       </c>
       <c r="P175" s="6">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="Q175" s="7">
         <v>3</v>
@@ -16232,10 +16242,10 @@
         <v>24</v>
       </c>
       <c r="J181" s="11">
-        <v>0.57291666666666663</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="K181" s="11">
-        <v>0.63472222222222219</v>
+        <v>0.41597222222222224</v>
       </c>
       <c r="L181">
         <v>1</v>
@@ -16244,7 +16254,7 @@
         <v>78</v>
       </c>
       <c r="N181" s="5">
-        <v>4700</v>
+        <v>4300</v>
       </c>
       <c r="O181" s="6">
         <v>-31.275107325818368</v>
@@ -17522,8 +17532,8 @@
       <c r="O198" s="6">
         <v>0</v>
       </c>
-      <c r="P198" s="6">
-        <v>1</v>
+      <c r="P198" s="12">
+        <v>50</v>
       </c>
       <c r="Q198" s="7">
         <v>2.4</v>
@@ -17676,8 +17686,8 @@
       <c r="O200" s="6">
         <v>0</v>
       </c>
-      <c r="P200" s="6">
-        <v>1</v>
+      <c r="P200" s="12">
+        <v>50</v>
       </c>
       <c r="U200" s="7" t="s">
         <v>413</v>
@@ -18143,8 +18153,8 @@
       <c r="O207" s="6">
         <v>0</v>
       </c>
-      <c r="P207" s="6">
-        <v>1</v>
+      <c r="P207" s="12">
+        <v>25</v>
       </c>
       <c r="U207" s="7" t="s">
         <v>447</v>
@@ -19987,8 +19997,8 @@
       <c r="O235" s="6">
         <v>0</v>
       </c>
-      <c r="P235" s="6">
-        <v>1</v>
+      <c r="P235" s="12">
+        <v>25</v>
       </c>
       <c r="Q235" s="7">
         <v>2.9</v>
@@ -20064,8 +20074,8 @@
       <c r="O236" s="6">
         <v>0</v>
       </c>
-      <c r="P236" s="6">
-        <v>1</v>
+      <c r="P236" s="12">
+        <v>25</v>
       </c>
       <c r="Q236" s="7">
         <v>2.9</v>
@@ -20095,8 +20105,67 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
+    <row r="237" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="C237" t="s">
+        <v>560</v>
+      </c>
+      <c r="D237" t="s">
+        <v>497</v>
+      </c>
+      <c r="E237" t="s">
+        <v>494</v>
+      </c>
+      <c r="F237" t="s">
+        <v>3</v>
+      </c>
+      <c r="G237" s="1">
+        <v>45312</v>
+      </c>
+      <c r="H237" s="1">
+        <v>45406</v>
+      </c>
+      <c r="I237" t="s">
+        <v>152</v>
+      </c>
+      <c r="J237" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="K237" s="11">
+        <v>0.56180555555555556</v>
+      </c>
+      <c r="L237">
+        <v>0.5</v>
+      </c>
+      <c r="M237">
+        <v>18</v>
+      </c>
+      <c r="N237" s="5">
+        <v>248</v>
+      </c>
+      <c r="O237" s="6">
+        <v>0</v>
+      </c>
+      <c r="P237" s="6">
+        <v>6</v>
+      </c>
+      <c r="Q237" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R237" s="7">
+        <v>2.6</v>
+      </c>
+      <c r="S237" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="T237" s="7">
+        <v>2.8</v>
+      </c>
+      <c r="U237" s="7" t="s">
+        <v>494</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="C1:AI236" xr:uid="{A458C66A-1996-8645-A24F-CDFC1D0B0EC5}"/>
+  <autoFilter ref="C1:AI237" xr:uid="{A458C66A-1996-8645-A24F-CDFC1D0B0EC5}"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>